<commit_message>
updated the input fields
</commit_message>
<xml_diff>
--- a/error_log.xlsx
+++ b/error_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -863,6 +863,2652 @@
         </is>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Warning</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Missing 'Comment' field in JSON object.</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>581</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>2025-04-09 01:04:33</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Warning</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>No answer found for question ID: smoker.cigarettes_per_day</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>390</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>2025-04-09 01:07:07</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Warning</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>No answer found for question ID: smoker.smoking_duration</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>390</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>2025-04-09 01:07:07</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Warning</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>No answer found for question ID: alcohol.drinks_per_week</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>390</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>2025-04-09 01:07:07</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Warning</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>No answer found for question ID: alcohol.alcohol_duration</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>390</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>2025-04-09 01:07:07</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Warning</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>No answer found for question ID: medications.medication_list</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>390</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>2025-04-09 01:07:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Warning</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>No answer found for question ID: medications.medication_duration</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>390</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>2025-04-09 01:07:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Warning</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>No answer found for question ID: medications.medication_side_effects</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>390</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>2025-04-09 01:07:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Warning</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>No answer found for question ID: appetite.decreased_appetite_reason</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>390</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>2025-04-09 01:07:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Warning</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>No answer found for question ID: appetite.weight_loss</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>390</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>2025-04-09 01:07:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Warning</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>No answer found for question ID: relationship_problems.relationship_type</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>390</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>2025-04-09 01:07:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Error</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>API Error: 404 - {
+  "id": "npJmg1Z-4yUbBN-92d437b70f8707c8",
+  "error": {
+    "message": "Unable to access model deepseek-ai/DeepSeek-R11. Please visit https://api.together.ai/models to view the list of supported models.",
+    "type": "invalid_request_error",
+    "param": null,
+    "code": "model_not_available"
+  }
+}</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>471</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>2025-04-09 01:07:09</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Warning</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>No answer found for question ID: smoker.cigarettes_per_day</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>406</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>2025-04-09 01:55:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Warning</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>No answer found for question ID: smoker.smoking_duration</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>406</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>2025-04-09 01:55:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Warning</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>No answer found for question ID: alcohol.drinks_per_week</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>406</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>2025-04-09 01:55:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Warning</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>No answer found for question ID: alcohol.alcohol_duration</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>406</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>2025-04-09 01:55:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Warning</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>No answer found for question ID: medications.medication_list</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>406</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>2025-04-09 01:55:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Warning</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>No answer found for question ID: medications.medication_duration</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>406</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>2025-04-09 01:55:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Warning</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>No answer found for question ID: medications.medication_side_effects</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>406</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>2025-04-09 01:55:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Warning</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>No answer found for question ID: appetite.decreased_appetite_reason</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>406</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>2025-04-09 01:55:03</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Warning</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>No answer found for question ID: appetite.weight_loss</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>406</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>2025-04-09 01:55:03</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Error</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>API Error: 404 - {
+  "id": "npK2QXW-4yUbBN-92d47de59d0af284",
+  "error": {
+    "message": "Unable to access model deepseek-ai/DeepSeek-R11. Please visit https://api.together.ai/models to view the list of supported models.",
+    "type": "invalid_request_error",
+    "param": null,
+    "code": "model_not_available"
+  }
+}</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>502</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>2025-04-09 01:55:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Warning</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Missing 'Comment' field in JSON object.</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>612</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>2025-04-09 17:07:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Warning</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>No answer found for question ID: smoker.cigarettes_per_day</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>406</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>2025-04-09 17:13:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Warning</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>No answer found for question ID: smoker.smoking_duration</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>406</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>2025-04-09 17:13:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Warning</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>No answer found for question ID: alcohol.drinks_per_week</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>406</v>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>2025-04-09 17:13:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Warning</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>No answer found for question ID: alcohol.alcohol_duration</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>406</v>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>2025-04-09 17:13:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Warning</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>No answer found for question ID: medications.medication_list</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>406</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>2025-04-09 17:13:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Warning</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>No answer found for question ID: medications.medication_duration</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>406</v>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>2025-04-09 17:13:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Warning</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>No answer found for question ID: medications.medication_side_effects</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>406</v>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>2025-04-09 17:13:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Warning</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>No answer found for question ID: appetite.decreased_appetite_reason</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>406</v>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>2025-04-09 17:13:05</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Warning</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>No answer found for question ID: appetite.weight_loss</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>406</v>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>2025-04-09 17:13:05</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Warning</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>No answer found for question ID: relationship_problems.relationship_type</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>406</v>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>2025-04-09 17:13:05</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Error</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>API Error: 404 - {
+  "id": "npPtiW5-4yUbBN-92d9beac7a3d3b72",
+  "error": {
+    "message": "Unable to access model deepseek-ai/DeepSeek-R11. Please visit https://api.together.ai/models to view the list of supported models.",
+    "type": "invalid_request_error",
+    "param": null,
+    "code": "model_not_available"
+  }
+}</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>502</v>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>2025-04-09 17:13:06</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Warning</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>No answer found for question ID: medications.medication_list</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>406</v>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>2025-04-09 17:41:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Warning</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>No answer found for question ID: medications.medication_duration</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>406</v>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>2025-04-09 17:41:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Warning</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>No answer found for question ID: medications.medication_side_effects</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>406</v>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>2025-04-09 17:41:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Warning</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>No answer found for question ID: energy</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>406</v>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>2025-04-09 17:41:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Warning</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>No answer found for question ID: social</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>406</v>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>2025-04-09 17:41:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Warning</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>No answer found for question ID: appetite</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>406</v>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>2025-04-09 17:41:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Warning</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>No answer found for question ID: mood</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>406</v>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>2025-04-09 17:41:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Warning</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>No answer found for question ID: relationship_problems</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>406</v>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>2025-04-09 17:41:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Error</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>API Error: 404 - {
+  "id": "npQ3U39-4yUbBN-92d9e85b4fd42010",
+  "error": {
+    "message": "Unable to access model deepseek-ai/DeepSeek-R11. Please visit https://api.together.ai/models to view the list of supported models.",
+    "type": "invalid_request_error",
+    "param": null,
+    "code": "model_not_available"
+  }
+}</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>502</v>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>2025-04-09 17:41:33</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Error</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Error converting user responses: string indices must be integers, not 'str'</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>351</v>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>2025-04-09 18:20:33</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Warning</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>No answer found for question ID: user_name</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>387</v>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>2025-04-09 18:20:33</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Warning</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>No answer found for question ID: user_type</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>387</v>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>2025-04-09 18:20:33</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Warning</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>No answer found for question ID: Date_of_Birth</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>387</v>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>2025-04-09 18:20:33</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Warning</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>No answer found for question ID: person_age</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>387</v>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>2025-04-09 18:20:33</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Warning</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>No answer found for question ID: concentration</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>387</v>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>2025-04-09 18:20:34</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Warning</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>No answer found for question ID: energy</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>387</v>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>2025-04-09 18:20:34</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Warning</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>No answer found for question ID: social</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>387</v>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>2025-04-09 18:20:34</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Warning</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>No answer found for question ID: mood</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>387</v>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>2025-04-09 18:20:34</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Warning</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>No answers were processed from user_responses.</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>412</v>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>2025-04-09 18:20:34</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Error</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>API Error: 404 - {
+  "id": "npQFUBN-4yUbBN-92da2187c80505bc",
+  "error": {
+    "message": "Unable to access model deepseek-ai/DeepSeek-R11. Please visit https://api.together.ai/models to view the list of supported models.",
+    "type": "invalid_request_error",
+    "param": null,
+    "code": "model_not_available"
+  }
+}</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>485</v>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>2025-04-09 18:20:35</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Warning</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>No answer found for question ID: medications.medication_list</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>406</v>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>2025-04-09 20:41:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Warning</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>No answer found for question ID: medications.medication_duration</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>406</v>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>2025-04-09 20:41:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Warning</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>No answer found for question ID: medications.medication_side_effects</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>406</v>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>2025-04-09 20:41:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Warning</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>No answer found for question ID: energy</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>406</v>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>2025-04-09 20:41:24</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Warning</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>No answer found for question ID: social</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>406</v>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>2025-04-09 20:41:24</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Warning</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>No answer found for question ID: appetite</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>406</v>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>2025-04-09 20:41:24</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Warning</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>No answer found for question ID: mood</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>406</v>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>2025-04-09 20:41:24</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Warning</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>No answer found for question ID: relationship_problems</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>406</v>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>2025-04-09 20:41:24</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>Error</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>API Error: 404 - {
+  "id": "npQznJQ-4yUbBN-92daefd90c190836",
+  "error": {
+    "message": "Unable to access model deepseek-ai/DeepSeek-R11. Please visit https://api.together.ai/models to view the list of supported models.",
+    "type": "invalid_request_error",
+    "param": null,
+    "code": "model_not_available"
+  }
+}</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>502</v>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>2025-04-09 20:41:26</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>Warning</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>No answer found for question ID: smoker.cigarettes_per_day</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>394</v>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>2025-04-10 00:34:18</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>Warning</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>No answer found for question ID: smoker.smoking_duration</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>394</v>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>2025-04-10 00:34:18</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>Warning</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>No answer found for question ID: alcohol.drinks_per_week</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>394</v>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>2025-04-10 00:34:18</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>Warning</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>No answer found for question ID: alcohol.alcohol_duration</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>394</v>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>2025-04-10 00:34:18</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>Warning</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>No answer found for question ID: medications.medication_list</t>
+        </is>
+      </c>
+      <c r="D80" t="n">
+        <v>394</v>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>2025-04-10 00:34:18</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>Warning</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>No answer found for question ID: medications.medication_duration</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>394</v>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>2025-04-10 00:34:19</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>Warning</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>No answer found for question ID: medications.medication_side_effects</t>
+        </is>
+      </c>
+      <c r="D82" t="n">
+        <v>394</v>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>2025-04-10 00:34:19</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>Warning</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>No answer found for question ID: appetite.decreased_appetite_reason</t>
+        </is>
+      </c>
+      <c r="D83" t="n">
+        <v>394</v>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>2025-04-10 00:34:19</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>Warning</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>No answer found for question ID: appetite.weight_loss</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>394</v>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>2025-04-10 00:34:19</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>Warning</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>No answer found for question ID: relationship_problems.relationship_type</t>
+        </is>
+      </c>
+      <c r="D85" t="n">
+        <v>394</v>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>2025-04-10 00:34:19</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>Mananow.py</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>Error</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>API Error: 404 - {
+  "id": "npSEQPZ-4yUbBN-92dc450489fa81d5",
+  "error": {
+    "message": "Unable to access model deepseek-ai/DeepSeek-R11. Please visit https://api.together.ai/models to view the list of supported models.",
+    "type": "invalid_request_error",
+    "param": null,
+    "code": "model_not_available"
+  }
+}</t>
+        </is>
+      </c>
+      <c r="D86" t="n">
+        <v>474</v>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>2025-04-10 00:34:20</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>